<commit_message>
Results of lab #01
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="23955" windowHeight="12780"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="23955" windowHeight="12780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="263929" sheetId="3" r:id="rId1"/>
@@ -18,8 +18,152 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>stas</author>
+  </authors>
+  <commentList>
+    <comment ref="E18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>stas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Хозяйский IP
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>stas</author>
+  </authors>
+  <commentList>
+    <comment ref="E11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>stas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Чужой IP
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>stas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Чужой IP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>stas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Беда с IP
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>stas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Беда с IP
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="183">
   <si>
     <t>Текущая аттестация 1.0</t>
   </si>
@@ -678,12 +822,15 @@
   <si>
     <t>53612707</t>
   </si>
+  <si>
+    <t>~</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -885,6 +1032,19 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1267,10 +1427,10 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1614,11 +1774,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1873,7 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8"/>
@@ -1929,7 +2089,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>5</v>
@@ -2104,7 +2264,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>5</v>
@@ -2314,7 +2474,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>5</v>
@@ -2489,7 +2649,7 @@
         <v>20</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>5</v>
@@ -2559,7 +2719,7 @@
         <v>20</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>5</v>
@@ -2594,7 +2754,7 @@
         <v>20</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>5</v>
@@ -2629,7 +2789,7 @@
         <v>20</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>5</v>
@@ -2734,7 +2894,7 @@
         <v>20</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>5</v>
@@ -2769,7 +2929,7 @@
         <v>20</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>5</v>
@@ -2837,6 +2997,7 @@
     <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2880,7 +3041,7 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8"/>
@@ -2890,7 +3051,7 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8"/>
@@ -3837,11 +3998,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3936,7 +4097,7 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8"/>
@@ -3946,7 +4107,7 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="8"/>
@@ -4081,8 +4242,9 @@
       <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>5</v>
+      <c r="E11" s="4" t="str">
+        <f>"+?"</f>
+        <v>+?</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>5</v>
@@ -4152,7 +4314,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>5</v>
@@ -4187,7 +4349,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>5</v>
@@ -4222,7 +4384,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>5</v>
@@ -4362,7 +4524,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>5</v>
@@ -4397,7 +4559,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>5</v>
@@ -4432,7 +4594,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>5</v>
@@ -4502,7 +4664,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>5</v>
@@ -4642,7 +4804,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>5</v>
+        <v>182</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>5</v>
@@ -4712,7 +4874,7 @@
         <v>20</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>5</v>
@@ -4817,7 +4979,7 @@
         <v>20</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>5</v>
@@ -4885,5 +5047,6 @@
     <mergeCell ref="B6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>